<commit_message>
Building up the class functionality.
next up is prioritizing items and refreshing the priority queues.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA96E95-309E-4E84-8404-72E51AEFEA30}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA59E70-4610-4B02-8114-43FE352E1892}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -62,6 +62,21 @@
   </si>
   <si>
     <t>Design + Building Classes</t>
+  </si>
+  <si>
+    <t>Wk [11] Sunday 27.5.18</t>
+  </si>
+  <si>
+    <t>Designing Factory Class + Stats + Item</t>
+  </si>
+  <si>
+    <t>1200 - 1530</t>
+  </si>
+  <si>
+    <t>1700 - 1800</t>
+  </si>
+  <si>
+    <t>Designing Stages</t>
   </si>
 </sst>
 </file>
@@ -69,8 +84,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="[$-C09]dddd\,\ d\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="[$-C09]dddd\,\ d\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -117,10 +132,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -129,7 +144,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -139,6 +153,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -161,10 +176,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A90FC5F8-4544-4D0D-9FA4-F5678436F556}" name="Table1" displayName="Table1" ref="A1:D16" totalsRowShown="0" dataDxfId="4">
   <autoFilter ref="A1:D16" xr:uid="{8FFAF145-D05C-4D40-85F8-11DC3C07801E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A6C54378-A635-4BFE-9A30-6C0546A6B7A5}" name="Date" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{D6724FE4-E1F3-48D5-A850-5C81059B21DE}" name="Time" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{90392D3D-45AB-4259-98B7-C74468C43BA0}" name="Hours" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{C46D515F-1A63-4F6F-B036-71F4FE15781A}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A6C54378-A635-4BFE-9A30-6C0546A6B7A5}" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D6724FE4-E1F3-48D5-A850-5C81059B21DE}" name="Time" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{90392D3D-45AB-4259-98B7-C74468C43BA0}" name="Hours" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C46D515F-1A63-4F6F-B036-71F4FE15781A}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -436,7 +451,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,23 +512,39 @@
         <v>12</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
@@ -576,7 +607,7 @@
       </c>
       <c r="C16" s="2">
         <f>SUBTOTAL(109,C2:C15)</f>
-        <v>6.33</v>
+        <v>8.83</v>
       </c>
       <c r="D16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Starting implementing simple structure.
Need to work out a system of refreshing the states and the queues. Possibly will be integrated or they will be causal. One after the other. Refresh either queues or stages one at a time or refresh them together.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA59E70-4610-4B02-8114-43FE352E1892}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAA5141-0220-4BFC-A43D-BF44C560FCC1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>Designing Stages</t>
+  </si>
+  <si>
+    <t>Implementing Priority Queues</t>
+  </si>
+  <si>
+    <t>Wk [12] Monday 28.5.18</t>
+  </si>
+  <si>
+    <t>1700 - 2100</t>
   </si>
 </sst>
 </file>
@@ -451,7 +460,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,10 +556,18 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -607,7 +624,7 @@
       </c>
       <c r="C16" s="2">
         <f>SUBTOTAL(109,C2:C15)</f>
-        <v>8.83</v>
+        <v>12.83</v>
       </c>
       <c r="D16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Refer to book for what to test next.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAA5141-0220-4BFC-A43D-BF44C560FCC1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1428EBDC-49E3-45E5-86B6-034C641B8FA0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>1700 - 2100</t>
+  </si>
+  <si>
+    <t>2300 - 0100</t>
+  </si>
+  <si>
+    <t>Joining the structures together</t>
+  </si>
+  <si>
+    <t>Wk[12] Wednesday 30.5.18</t>
   </si>
 </sst>
 </file>
@@ -460,7 +469,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,10 +579,18 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -624,7 +641,7 @@
       </c>
       <c r="C16" s="2">
         <f>SUBTOTAL(109,C2:C15)</f>
-        <v>12.83</v>
+        <v>14.83</v>
       </c>
       <c r="D16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Implementing the updater of the factory.
Tricky but braybray has given me the confidence to continue.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1428EBDC-49E3-45E5-86B6-034C641B8FA0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F62AB91-E0F1-48EA-A989-A56D3D8174A5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>Wk[12] Wednesday 30.5.18</t>
+  </si>
+  <si>
+    <t>Wk[12] Thursday 31.5.18</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>1700 - 2130</t>
   </si>
 </sst>
 </file>
@@ -469,7 +478,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,10 +602,18 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -641,7 +658,7 @@
       </c>
       <c r="C16" s="2">
         <f>SUBTOTAL(109,C2:C15)</f>
-        <v>14.83</v>
+        <v>19.329999999999998</v>
       </c>
       <c r="D16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Debugging logic of updateFactory()
Just keep chipping away. It will work. Remember to draw things out as well.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F62AB91-E0F1-48EA-A989-A56D3D8174A5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB12315-CBA9-41EA-AB58-2FBD32F868AD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -100,10 +100,19 @@
     <t>Wk[12] Thursday 31.5.18</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>1700 - 2130</t>
+  </si>
+  <si>
+    <t>Wk[12] Friday 1.6.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1400 - 1700 </t>
+  </si>
+  <si>
+    <t>Testing simple structure (2 stages 1 queue).</t>
+  </si>
+  <si>
+    <t>Implementing interactions between more complex structures.</t>
   </si>
 </sst>
 </file>
@@ -478,7 +487,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,20 +615,28 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1">
         <v>4.5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -658,7 +675,7 @@
       </c>
       <c r="C16" s="2">
         <f>SUBTOTAL(109,C2:C15)</f>
-        <v>19.329999999999998</v>
+        <v>22.33</v>
       </c>
       <c r="D16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Starting to implement statistics. Doing a rework of updateFactory.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB12315-CBA9-41EA-AB58-2FBD32F868AD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D68327-3C92-4C36-AC34-EEAF8D6F1001}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>Implementing interactions between more complex structures.</t>
+  </si>
+  <si>
+    <t>Wk[12] Saturday 2.6.18</t>
+  </si>
+  <si>
+    <t>1300  - 1600</t>
+  </si>
+  <si>
+    <t>Reparing logic of updating the facotry</t>
   </si>
 </sst>
 </file>
@@ -487,7 +496,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,10 +648,18 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -675,7 +692,7 @@
       </c>
       <c r="C16" s="2">
         <f>SUBTOTAL(109,C2:C15)</f>
-        <v>22.33</v>
+        <v>25.33</v>
       </c>
       <c r="D16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Cleaned up code significantly. Starting to collect statistics.
Still needs more cleaning but getting there. Confidence building. It will be okay.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D68327-3C92-4C36-AC34-EEAF8D6F1001}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A79E71-91FE-4171-ADD8-A78543708853}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>Reparing logic of updating the facotry</t>
+  </si>
+  <si>
+    <t>1600 - 2300</t>
+  </si>
+  <si>
+    <t>Improving readability of code. It was so bad.</t>
   </si>
 </sst>
 </file>
@@ -496,7 +502,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,10 +668,18 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
@@ -692,7 +706,7 @@
       </c>
       <c r="C16" s="2">
         <f>SUBTOTAL(109,C2:C15)</f>
-        <v>25.33</v>
+        <v>30.33</v>
       </c>
       <c r="D16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Still stujck on blocking.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A79E71-91FE-4171-ADD8-A78543708853}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1A533F-BB89-4CB4-B011-A5DD8B1E2C8E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t>Improving readability of code. It was so bad.</t>
+  </si>
+  <si>
+    <t>Wk[12] Sunday 3.6.18</t>
+  </si>
+  <si>
+    <t>1200 - 1200</t>
+  </si>
+  <si>
+    <t>Debugging blocking logic.</t>
   </si>
 </sst>
 </file>
@@ -502,7 +511,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,10 +691,18 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -706,7 +723,7 @@
       </c>
       <c r="C16" s="2">
         <f>SUBTOTAL(109,C2:C15)</f>
-        <v>30.33</v>
+        <v>42.33</v>
       </c>
       <c r="D16" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added report and some shiznit. Now I'm really going to mess with logic.
</commit_message>
<xml_diff>
--- a/TimeTrack.xlsx
+++ b/TimeTrack.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1A533F-BB89-4CB4-B011-A5DD8B1E2C8E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABF7558-7E80-453A-B7BC-7AAAECD43016}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -40,18 +40,12 @@
     <t xml:space="preserve">1600 - 1800 </t>
   </si>
   <si>
-    <t xml:space="preserve">Spec Breakdown </t>
-  </si>
-  <si>
     <t>[Wk 11] Thursday 24.5.18</t>
   </si>
   <si>
     <t>[Wk 11] Monday 21.5.18</t>
   </si>
   <si>
-    <t>Research into discrete time simulations</t>
-  </si>
-  <si>
     <t xml:space="preserve">1850 - 1910 </t>
   </si>
   <si>
@@ -61,27 +55,15 @@
     <t>1300 - 1800</t>
   </si>
   <si>
-    <t>Design + Building Classes</t>
-  </si>
-  <si>
     <t>Wk [11] Sunday 27.5.18</t>
   </si>
   <si>
-    <t>Designing Factory Class + Stats + Item</t>
-  </si>
-  <si>
     <t>1200 - 1530</t>
   </si>
   <si>
     <t>1700 - 1800</t>
   </si>
   <si>
-    <t>Designing Stages</t>
-  </si>
-  <si>
-    <t>Implementing Priority Queues</t>
-  </si>
-  <si>
     <t>Wk [12] Monday 28.5.18</t>
   </si>
   <si>
@@ -91,9 +73,6 @@
     <t>2300 - 0100</t>
   </si>
   <si>
-    <t>Joining the structures together</t>
-  </si>
-  <si>
     <t>Wk[12] Wednesday 30.5.18</t>
   </si>
   <si>
@@ -109,34 +88,82 @@
     <t xml:space="preserve">1400 - 1700 </t>
   </si>
   <si>
-    <t>Testing simple structure (2 stages 1 queue).</t>
-  </si>
-  <si>
-    <t>Implementing interactions between more complex structures.</t>
-  </si>
-  <si>
     <t>Wk[12] Saturday 2.6.18</t>
   </si>
   <si>
     <t>1300  - 1600</t>
   </si>
   <si>
-    <t>Reparing logic of updating the facotry</t>
-  </si>
-  <si>
     <t>1600 - 2300</t>
   </si>
   <si>
-    <t>Improving readability of code. It was so bad.</t>
-  </si>
-  <si>
     <t>Wk[12] Sunday 3.6.18</t>
   </si>
   <si>
-    <t>1200 - 1200</t>
-  </si>
-  <si>
-    <t>Debugging blocking logic.</t>
+    <t>Spec Breakdown [DESIGN]</t>
+  </si>
+  <si>
+    <t>Research into discrete time simulations [DESIGN]</t>
+  </si>
+  <si>
+    <t>Design + Building Classes [DESIGN]</t>
+  </si>
+  <si>
+    <t>Designing Factory Class + Stats + Item [DESIGN]</t>
+  </si>
+  <si>
+    <t>Designing Stages [DESIGN]</t>
+  </si>
+  <si>
+    <t>Implementing Priority Queues [CODING]</t>
+  </si>
+  <si>
+    <t>Wk[13] Monday 4.6.18</t>
+  </si>
+  <si>
+    <t>1200 - 2400</t>
+  </si>
+  <si>
+    <t>2400 - 0300</t>
+  </si>
+  <si>
+    <t>Improving readability of code. It was so bad. [REVIEWING]</t>
+  </si>
+  <si>
+    <t>Joining the structures together [CODING]</t>
+  </si>
+  <si>
+    <t>Testing simple structure (2 stages 1 queue). [TESTING]</t>
+  </si>
+  <si>
+    <t>Implementing interactions between more complex structures. [CODING]</t>
+  </si>
+  <si>
+    <t>Reparing logic of updating the factory. [REVIEWING]</t>
+  </si>
+  <si>
+    <t>Debugging blocking logic. [CORRECTING]</t>
+  </si>
+  <si>
+    <t>DESIGNING</t>
+  </si>
+  <si>
+    <t>CORRECTING</t>
+  </si>
+  <si>
+    <t>CODING</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>REVIEWING</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Percentage of Time (%)</t>
   </si>
 </sst>
 </file>
@@ -184,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -198,11 +225,39 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -233,13 +288,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A90FC5F8-4544-4D0D-9FA4-F5678436F556}" name="Table1" displayName="Table1" ref="A1:D16" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A90FC5F8-4544-4D0D-9FA4-F5678436F556}" name="Table1" displayName="Table1" ref="A1:D16" totalsRowShown="0" dataDxfId="8">
   <autoFilter ref="A1:D16" xr:uid="{8FFAF145-D05C-4D40-85F8-11DC3C07801E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A6C54378-A635-4BFE-9A30-6C0546A6B7A5}" name="Date" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{D6724FE4-E1F3-48D5-A850-5C81059B21DE}" name="Time" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{90392D3D-45AB-4259-98B7-C74468C43BA0}" name="Hours" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{C46D515F-1A63-4F6F-B036-71F4FE15781A}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A6C54378-A635-4BFE-9A30-6C0546A6B7A5}" name="Date" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{D6724FE4-E1F3-48D5-A850-5C81059B21DE}" name="Time" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{90392D3D-45AB-4259-98B7-C74468C43BA0}" name="Hours" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{C46D515F-1A63-4F6F-B036-71F4FE15781A}" name="Description" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E346F930-6A0D-4A52-B4AA-3C974568949B}" name="Table2" displayName="Table2" ref="A18:B23" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="A18:B23" xr:uid="{DF60ADD1-265F-421D-8128-356368668BBA}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A34DFF87-0378-47C2-9BB1-8366EF5B5B4B}" name="Phase" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{FB2193BB-0D34-40C3-9344-B7772D95FE31}" name="Percentage of Time (%)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -508,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +588,7 @@
     <col min="4" max="4" width="77.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,9 +602,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -547,141 +613,146 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>0.33</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>3.5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1">
         <v>4.5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1">
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1">
         <v>5</v>
@@ -690,48 +761,113 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1">
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="2">
         <f>SUBTOTAL(109,C2:C15)</f>
-        <v>42.33</v>
+        <v>45.33</v>
       </c>
       <c r="D16" s="1"/>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="9">
+        <f>(2+0.33+2+3.5+1)/C16 *100</f>
+        <v>19.479373483344364</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="9">
+        <f>(4+2+3)/C16 *100</f>
+        <v>19.854401058901392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="9">
+        <f>4.5/C16 * 100</f>
+        <v>9.9272005294506958</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="9">
+        <f>8/C16 * 100</f>
+        <v>17.648356496801238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="9">
+        <f>15/C16 * 100</f>
+        <v>33.090668431502316</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:E6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>